<commit_message>
Updates to the MainPageTest.java file
</commit_message>
<xml_diff>
--- a/Spotify_Project/src/test/resources/testdata/Test_data.xlsx
+++ b/Spotify_Project/src/test/resources/testdata/Test_data.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12495" windowHeight="6060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:E9"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Test scenario</t>
   </si>
@@ -57,9 +58,6 @@
   </si>
   <si>
     <t xml:space="preserve">From the main page, click on the Help link and verify if the page loads correctly </t>
-  </si>
-  <si>
-    <t xml:space="preserve">From the main page, click on the Download link and verify if the page loads correctly </t>
   </si>
   <si>
     <t xml:space="preserve">From the main page, click on the Sign Up link and verify if the page loads correctly </t>
@@ -124,9 +122,6 @@
   </si>
   <si>
     <t xml:space="preserve">From the main page, click on the Spotify icon and verify if the page loads correctly </t>
-  </si>
-  <si>
-    <t>TS3TC006</t>
   </si>
   <si>
     <t>Aleksandra M</t>
@@ -696,9 +691,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -728,7 +723,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -753,7 +748,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="25"/>
       <c r="E4" s="13" t="s">
@@ -776,10 +771,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,16 +788,16 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>1</v>
@@ -812,107 +807,101 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>24</v>
-      </c>
       <c r="E4" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="19"/>
       <c r="C5" s="6"/>
       <c r="D5" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="19"/>
       <c r="C7" s="6"/>
       <c r="D7" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="19"/>
       <c r="C8" s="6"/>
       <c r="D8" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="19"/>
       <c r="C9" s="6"/>
       <c r="D9" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="19"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="20" t="s">
+    <row r="10" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="21"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>16</v>
-      </c>
+    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>